<commit_message>
pushing new changes for agilepoint & updates
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,11 @@
     <sheet name="Assets" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -119,18 +118,6 @@
     <t>FTP_Host</t>
   </si>
   <si>
-    <t>EmailSubjectJENotifySubmitter</t>
-  </si>
-  <si>
-    <t>EmailSubjectJEOutOfBalance</t>
-  </si>
-  <si>
-    <t>EmailSubjectJERequestApproval</t>
-  </si>
-  <si>
-    <t>EmailSubjectJSecurityRejection</t>
-  </si>
-  <si>
     <t>SupportingJEFilesPath</t>
   </si>
   <si>
@@ -141,6 +128,15 @@
   </si>
   <si>
     <t>\Documents\JE Files\JE Excel</t>
+  </si>
+  <si>
+    <t>SQLConnectionString</t>
+  </si>
+  <si>
+    <t>AgilePointCredentials</t>
+  </si>
+  <si>
+    <t>AgilePointServerURL</t>
   </si>
 </sst>
 </file>
@@ -527,7 +523,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -602,21 +598,28 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>38</v>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2726,10 +2729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2750,7 +2753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -2760,34 +2763,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
+      <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>